<commit_message>
week 10 - completed lab
</commit_message>
<xml_diff>
--- a/Week 10/data_processing_example/tableA1.xlsx
+++ b/Week 10/data_processing_example/tableA1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jatho\Documents\CCS\GRD610A-W21 Content\Week 10\data_processing_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C35C65B-CC66-40A5-8CD1-BA76D6BDEB19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FE4DF8-4CCD-4267-8357-45C06874DDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tableA1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Update2" sheetId="3" r:id="rId3"/>
     <sheet name="Update3" sheetId="4" r:id="rId4"/>
     <sheet name="Update4" sheetId="5" r:id="rId5"/>
+    <sheet name="Update5" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">tableA1!$A$1:$I$51</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="81">
   <si>
     <t>Table with row headers in column A and column headers in rows 4 through 6</t>
   </si>
@@ -781,6 +782,15 @@
   </si>
   <si>
     <t>Median_Income_2019</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Count Thousands</t>
+  </si>
+  <si>
+    <t>Median Income</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1095,9 +1105,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1127,18 +1134,16 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1165,10 +1170,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1510,42 +1526,42 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="9" width="11.5703125" customWidth="1"/>
+    <col min="2" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-    </row>
-    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-    </row>
-    <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
@@ -1558,54 +1574,54 @@
       <c r="H3" s="33"/>
       <c r="I3" s="33"/>
     </row>
-    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="41">
         <v>2018</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41">
         <v>2019</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="40" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="41"/>
-    </row>
-    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
-      <c r="B5" s="37" t="s">
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35"/>
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="37" t="s">
+      <c r="D5" s="41"/>
+      <c r="E5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
-    </row>
-    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="40"/>
+    </row>
+    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1619,20 +1635,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -1661,20 +1677,20 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+    <row r="9" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1703,7 +1719,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1732,7 +1748,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -1761,7 +1777,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -1790,7 +1806,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1819,7 +1835,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1848,7 +1864,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1877,20 +1893,20 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A17" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>19</v>
       </c>
@@ -1919,7 +1935,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -1948,7 +1964,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1977,7 +1993,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -2006,7 +2022,7 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2035,20 +2051,20 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="32" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -2077,7 +2093,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>27</v>
       </c>
@@ -2106,7 +2122,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -2135,7 +2151,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>29</v>
       </c>
@@ -2164,7 +2180,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>30</v>
       </c>
@@ -2193,7 +2209,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>31</v>
       </c>
@@ -2222,7 +2238,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2251,20 +2267,20 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
@@ -2293,7 +2309,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
@@ -2322,7 +2338,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>35</v>
       </c>
@@ -2351,7 +2367,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
@@ -2380,20 +2396,20 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="32" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -2422,7 +2438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>39</v>
       </c>
@@ -2451,7 +2467,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -2480,7 +2496,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -2509,20 +2525,20 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="32" t="s">
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A41" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2551,7 +2567,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
@@ -2580,7 +2596,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>46</v>
       </c>
@@ -2609,7 +2625,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -2638,20 +2654,20 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-    </row>
-    <row r="47" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+    </row>
+    <row r="47" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>48</v>
       </c>
@@ -2664,7 +2680,7 @@
       <c r="H47" s="33"/>
       <c r="I47" s="33"/>
     </row>
-    <row r="48" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>49</v>
       </c>
@@ -2677,47 +2693,60 @@
       <c r="H48" s="33"/>
       <c r="I48" s="33"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+      <c r="H49" s="44"/>
+      <c r="I49" s="44"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A46:I46"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A31:I31"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
@@ -2729,19 +2758,6 @@
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A46:I46"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A48:I48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2758,61 +2774,61 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="44">
+      <c r="B1" s="47">
         <v>2018</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47">
         <v>2019</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="17" t="s">
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="18"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="44"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="44"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="G2" s="47"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
@@ -2825,7 +2841,7 @@
       <c r="D3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="30" t="s">
         <v>75</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2841,20 +2857,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-    </row>
-    <row r="5" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
@@ -2883,20 +2899,20 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+    </row>
+    <row r="7" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2925,7 +2941,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -2954,7 +2970,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -2983,7 +2999,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -3012,7 +3028,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -3041,7 +3057,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -3070,7 +3086,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
@@ -3099,20 +3115,20 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A14" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -3141,7 +3157,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
@@ -3170,7 +3186,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -3199,7 +3215,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -3228,7 +3244,7 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -3257,20 +3273,20 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -3299,7 +3315,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
@@ -3328,7 +3344,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
@@ -3357,7 +3373,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -3386,7 +3402,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -3415,7 +3431,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -3444,7 +3460,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -3473,20 +3489,20 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -3515,7 +3531,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -3544,7 +3560,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
@@ -3573,7 +3589,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>36</v>
       </c>
@@ -3602,20 +3618,20 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -3644,7 +3660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -3673,7 +3689,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -3702,7 +3718,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -3731,20 +3747,20 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="32" t="s">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A38" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+    </row>
+    <row r="39" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -3773,7 +3789,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>45</v>
       </c>
@@ -3802,7 +3818,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>46</v>
       </c>
@@ -3831,7 +3847,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -3861,11 +3877,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="7">
     <mergeCell ref="A38:I38"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A6:I6"/>
@@ -3883,23 +3895,23 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
@@ -3928,20 +3940,20 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -3970,20 +3982,20 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-    </row>
-    <row r="5" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+    </row>
+    <row r="5" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -4012,7 +4024,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -4041,7 +4053,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -4070,7 +4082,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -4099,7 +4111,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -4128,7 +4140,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4157,7 +4169,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -4186,20 +4198,20 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+    <row r="12" spans="1:9" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -4228,7 +4240,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
@@ -4257,7 +4269,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4286,7 +4298,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -4315,7 +4327,7 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -4344,20 +4356,20 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+    <row r="18" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -4386,7 +4398,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -4415,7 +4427,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
@@ -4444,7 +4456,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
@@ -4473,7 +4485,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
@@ -4502,7 +4514,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
@@ -4531,7 +4543,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -4560,20 +4572,20 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46" t="s">
+    <row r="26" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -4602,7 +4614,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -4631,7 +4643,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>35</v>
       </c>
@@ -4660,7 +4672,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>36</v>
       </c>
@@ -4689,20 +4701,20 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="46" t="s">
+    <row r="31" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="46"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="46"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -4731,7 +4743,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -4760,7 +4772,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
@@ -4789,7 +4801,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -4818,20 +4830,20 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+    <row r="36" spans="1:9" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="A36" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="46"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-    </row>
-    <row r="37" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="45"/>
+      <c r="C36" s="45"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+    </row>
+    <row r="37" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
@@ -4860,7 +4872,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>45</v>
       </c>
@@ -4889,7 +4901,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
@@ -4918,7 +4930,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -4966,52 +4978,52 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -5040,7 +5052,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -5069,8 +5081,8 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="3">
@@ -5098,7 +5110,7 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
@@ -5127,7 +5139,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -5156,7 +5168,7 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -5185,7 +5197,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
@@ -5214,7 +5226,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
@@ -5243,7 +5255,7 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -5272,7 +5284,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -5301,7 +5313,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -5330,7 +5342,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -5359,7 +5371,7 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -5388,7 +5400,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -5417,7 +5429,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -5446,7 +5458,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -5475,7 +5487,7 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -5504,7 +5516,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -5533,7 +5545,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -5562,7 +5574,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -5591,7 +5603,7 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>33</v>
       </c>
@@ -5620,7 +5632,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -5649,7 +5661,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -5678,7 +5690,7 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -5707,7 +5719,7 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -5736,7 +5748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -5765,7 +5777,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -5794,7 +5806,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -5823,7 +5835,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
@@ -5852,7 +5864,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>45</v>
       </c>
@@ -5881,7 +5893,7 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>46</v>
       </c>
@@ -5910,7 +5922,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -5948,54 +5960,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C607C476-5815-4614-8212-884C83FF4F27}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="10">
@@ -6023,8 +6035,8 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3">
@@ -6052,8 +6064,8 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="3">
@@ -6081,8 +6093,8 @@
         <v>1.53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="3">
@@ -6110,8 +6122,8 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="3">
@@ -6139,8 +6151,8 @@
         <v>5.05</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3">
@@ -6168,8 +6180,8 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="3">
@@ -6197,8 +6209,8 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="3">
@@ -6226,8 +6238,8 @@
         <v>3.13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="3">
@@ -6255,8 +6267,8 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>62</v>
       </c>
       <c r="B11" s="3">
@@ -6284,8 +6296,8 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3">
@@ -6313,8 +6325,8 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B13" s="3">
@@ -6342,8 +6354,8 @@
         <v>5.24</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="3">
@@ -6371,8 +6383,8 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="3">
@@ -6400,8 +6412,8 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="3">
@@ -6429,8 +6441,8 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
         <v>64</v>
       </c>
       <c r="B17" s="3">
@@ -6458,8 +6470,8 @@
         <v>2.42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="30" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
         <v>65</v>
       </c>
       <c r="B18" s="3">
@@ -6487,8 +6499,8 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
         <v>66</v>
       </c>
       <c r="B19" s="3">
@@ -6516,8 +6528,8 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
         <v>67</v>
       </c>
       <c r="B20" s="3">
@@ -6545,8 +6557,8 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="3">
@@ -6574,8 +6586,8 @@
         <v>2.57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="3">
@@ -6603,8 +6615,8 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="3">
@@ -6632,8 +6644,8 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="3">
@@ -6661,8 +6673,8 @@
         <v>4.6900000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
         <v>69</v>
       </c>
       <c r="B25" s="3">
@@ -6690,8 +6702,8 @@
         <v>4.9400000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="3">
@@ -6719,8 +6731,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="3">
@@ -6748,8 +6760,8 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="3">
@@ -6777,8 +6789,8 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="3">
@@ -6806,8 +6818,8 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B30" s="3">
@@ -6835,8 +6847,8 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
         <v>70</v>
       </c>
       <c r="B31" s="3">
@@ -6864,8 +6876,8 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="30" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="3">
@@ -6893,8 +6905,8 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="3">
@@ -6920,6 +6932,936 @@
       </c>
       <c r="I33" s="5">
         <v>2.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F110A0-EC52-470F-B599-EDE8CCE7C355}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2018</v>
+      </c>
+      <c r="C2">
+        <v>128579</v>
+      </c>
+      <c r="D2">
+        <v>64324</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>2018</v>
+      </c>
+      <c r="C3">
+        <v>83482</v>
+      </c>
+      <c r="D3">
+        <v>82124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>2018</v>
+      </c>
+      <c r="C4">
+        <v>61959</v>
+      </c>
+      <c r="D4">
+        <v>95351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>2018</v>
+      </c>
+      <c r="C5">
+        <v>15043</v>
+      </c>
+      <c r="D5">
+        <v>45946</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>2018</v>
+      </c>
+      <c r="C6">
+        <v>6480</v>
+      </c>
+      <c r="D6">
+        <v>62632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>2018</v>
+      </c>
+      <c r="C7">
+        <v>45096</v>
+      </c>
+      <c r="D7">
+        <v>38813</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <v>2018</v>
+      </c>
+      <c r="C8">
+        <v>23515</v>
+      </c>
+      <c r="D8">
+        <v>32587</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9">
+        <v>2018</v>
+      </c>
+      <c r="C9">
+        <v>21582</v>
+      </c>
+      <c r="D9">
+        <v>46583</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>2018</v>
+      </c>
+      <c r="C10">
+        <v>100528</v>
+      </c>
+      <c r="D10">
+        <v>68156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11">
+        <v>84727</v>
+      </c>
+      <c r="D11">
+        <v>71922</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2018</v>
+      </c>
+      <c r="C12">
+        <v>17167</v>
+      </c>
+      <c r="D12">
+        <v>42110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>2018</v>
+      </c>
+      <c r="C13">
+        <v>6981</v>
+      </c>
+      <c r="D13">
+        <v>88774</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>2018</v>
+      </c>
+      <c r="C14">
+        <v>17758</v>
+      </c>
+      <c r="D14">
+        <v>52382</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>2018</v>
+      </c>
+      <c r="C15">
+        <v>94423</v>
+      </c>
+      <c r="D15">
+        <v>72958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>2018</v>
+      </c>
+      <c r="C16">
+        <v>6199</v>
+      </c>
+      <c r="D16">
+        <v>44320</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>2018</v>
+      </c>
+      <c r="C17">
+        <v>20611</v>
+      </c>
+      <c r="D17">
+        <v>67084</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>2018</v>
+      </c>
+      <c r="C18">
+        <v>21370</v>
+      </c>
+      <c r="D18">
+        <v>82206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>2018</v>
+      </c>
+      <c r="C19">
+        <v>22071</v>
+      </c>
+      <c r="D19">
+        <v>85994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20">
+        <v>2018</v>
+      </c>
+      <c r="C20">
+        <v>24172</v>
+      </c>
+      <c r="D20">
+        <v>70200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>2018</v>
+      </c>
+      <c r="C21">
+        <v>34156</v>
+      </c>
+      <c r="D21">
+        <v>44487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>2018</v>
+      </c>
+      <c r="C22">
+        <v>108560</v>
+      </c>
+      <c r="D22">
+        <v>65407</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>2018</v>
+      </c>
+      <c r="C23">
+        <v>20019</v>
+      </c>
+      <c r="D23">
+        <v>59841</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24">
+        <v>2018</v>
+      </c>
+      <c r="C24">
+        <v>11043</v>
+      </c>
+      <c r="D24">
+        <v>66707</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25">
+        <v>2018</v>
+      </c>
+      <c r="C25">
+        <v>8976</v>
+      </c>
+      <c r="D25">
+        <v>52885</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>2018</v>
+      </c>
+      <c r="C26">
+        <v>22054</v>
+      </c>
+      <c r="D26">
+        <v>71383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>2018</v>
+      </c>
+      <c r="C27">
+        <v>27686</v>
+      </c>
+      <c r="D27">
+        <v>65230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>2018</v>
+      </c>
+      <c r="C28">
+        <v>49743</v>
+      </c>
+      <c r="D28">
+        <v>58337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>2018</v>
+      </c>
+      <c r="C29">
+        <v>29096</v>
+      </c>
+      <c r="D29">
+        <v>70779</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>2018</v>
+      </c>
+      <c r="C30">
+        <v>110789</v>
+      </c>
+      <c r="D30">
+        <v>67363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31">
+        <v>2018</v>
+      </c>
+      <c r="C31">
+        <v>42983</v>
+      </c>
+      <c r="D31">
+        <v>60434</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32">
+        <v>2018</v>
+      </c>
+      <c r="C32">
+        <v>67806</v>
+      </c>
+      <c r="D32">
+        <v>72213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>2018</v>
+      </c>
+      <c r="C33">
+        <v>17790</v>
+      </c>
+      <c r="D33">
+        <v>50771</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>2019</v>
+      </c>
+      <c r="C34" s="10">
+        <v>128451</v>
+      </c>
+      <c r="D34" s="10">
+        <v>68703</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2019</v>
+      </c>
+      <c r="C35" s="3">
+        <v>83677</v>
+      </c>
+      <c r="D35" s="3">
+        <v>88149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36">
+        <v>2019</v>
+      </c>
+      <c r="C36" s="3">
+        <v>62342</v>
+      </c>
+      <c r="D36" s="3">
+        <v>102308</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37">
+        <v>2019</v>
+      </c>
+      <c r="C37" s="3">
+        <v>14832</v>
+      </c>
+      <c r="D37" s="3">
+        <v>48098</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38">
+        <v>2019</v>
+      </c>
+      <c r="C38" s="3">
+        <v>6503</v>
+      </c>
+      <c r="D38" s="3">
+        <v>69244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>2019</v>
+      </c>
+      <c r="C39" s="3">
+        <v>44774</v>
+      </c>
+      <c r="D39" s="3">
+        <v>41232</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40">
+        <v>2019</v>
+      </c>
+      <c r="C40" s="3">
+        <v>23470</v>
+      </c>
+      <c r="D40" s="3">
+        <v>34612</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41">
+        <v>2019</v>
+      </c>
+      <c r="C41" s="3">
+        <v>21304</v>
+      </c>
+      <c r="D41" s="3">
+        <v>48496</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42">
+        <v>2019</v>
+      </c>
+      <c r="C42" s="3">
+        <v>100568</v>
+      </c>
+      <c r="D42" s="3">
+        <v>72204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43">
+        <v>2019</v>
+      </c>
+      <c r="C43" s="3">
+        <v>84868</v>
+      </c>
+      <c r="D43" s="3">
+        <v>76057</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>2019</v>
+      </c>
+      <c r="C44" s="3">
+        <v>17054</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45438</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45">
+        <v>2019</v>
+      </c>
+      <c r="C45" s="3">
+        <v>6853</v>
+      </c>
+      <c r="D45" s="3">
+        <v>98174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46">
+        <v>2019</v>
+      </c>
+      <c r="C46" s="3">
+        <v>17667</v>
+      </c>
+      <c r="D46" s="3">
+        <v>56113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>2019</v>
+      </c>
+      <c r="C47" s="3">
+        <v>93524</v>
+      </c>
+      <c r="D47" s="3">
+        <v>77873</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48">
+        <v>2019</v>
+      </c>
+      <c r="C48" s="3">
+        <v>5406</v>
+      </c>
+      <c r="D48" s="3">
+        <v>47934</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49">
+        <v>2019</v>
+      </c>
+      <c r="C49" s="3">
+        <v>20424</v>
+      </c>
+      <c r="D49" s="3">
+        <v>70283</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50">
+        <v>2019</v>
+      </c>
+      <c r="C50" s="3">
+        <v>21432</v>
+      </c>
+      <c r="D50" s="3">
+        <v>88858</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51">
+        <v>2019</v>
+      </c>
+      <c r="C51" s="3">
+        <v>21659</v>
+      </c>
+      <c r="D51" s="3">
+        <v>92221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52">
+        <v>2019</v>
+      </c>
+      <c r="C52" s="3">
+        <v>24603</v>
+      </c>
+      <c r="D52" s="3">
+        <v>75686</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53">
+        <v>2019</v>
+      </c>
+      <c r="C53" s="3">
+        <v>34927</v>
+      </c>
+      <c r="D53" s="3">
+        <v>47357</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54">
+        <v>2019</v>
+      </c>
+      <c r="C54" s="3">
+        <v>108851</v>
+      </c>
+      <c r="D54" s="3">
+        <v>69474</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55">
+        <v>2019</v>
+      </c>
+      <c r="C55" s="3">
+        <v>19600</v>
+      </c>
+      <c r="D55" s="3">
+        <v>64900</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56">
+        <v>2019</v>
+      </c>
+      <c r="C56" s="3">
+        <v>11208</v>
+      </c>
+      <c r="D56" s="3">
+        <v>71538</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57">
+        <v>2019</v>
+      </c>
+      <c r="C57" s="3">
+        <v>8392</v>
+      </c>
+      <c r="D57" s="3">
+        <v>57668</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58">
+        <v>2019</v>
+      </c>
+      <c r="C58" s="3">
+        <v>22031</v>
+      </c>
+      <c r="D58" s="3">
+        <v>76221</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59">
+        <v>2019</v>
+      </c>
+      <c r="C59" s="3">
+        <v>27757</v>
+      </c>
+      <c r="D59" s="3">
+        <v>68354</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60">
+        <v>2019</v>
+      </c>
+      <c r="C60" s="3">
+        <v>49486</v>
+      </c>
+      <c r="D60" s="3">
+        <v>61884</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61">
+        <v>2019</v>
+      </c>
+      <c r="C61" s="3">
+        <v>29177</v>
+      </c>
+      <c r="D61" s="3">
+        <v>75769</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>2019</v>
+      </c>
+      <c r="C62" s="3">
+        <v>110679</v>
+      </c>
+      <c r="D62" s="3">
+        <v>71961</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63">
+        <v>2019</v>
+      </c>
+      <c r="C63" s="3">
+        <v>42992</v>
+      </c>
+      <c r="D63" s="3">
+        <v>63745</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64">
+        <v>2019</v>
+      </c>
+      <c r="C64" s="3">
+        <v>67687</v>
+      </c>
+      <c r="D64" s="3">
+        <v>77170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65">
+        <v>2019</v>
+      </c>
+      <c r="C65" s="3">
+        <v>17772</v>
+      </c>
+      <c r="D65" s="3">
+        <v>52100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>